<commit_message>
Updated Test Report and comment in ContentProviderTests.java
</commit_message>
<xml_diff>
--- a/doc/_editable/Test Report.xlsx
+++ b/doc/_editable/Test Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.clark\Desktop\GitHub2\WYSIWYD\doc\_editable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlgren\workspace\git\WYSIWYD\doc\_editable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Testcase</t>
   </si>
@@ -33,6 +33,96 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>testDeletes() sub-test 1</t>
+  </si>
+  <si>
+    <t>testDeletes() sub-test 2</t>
+  </si>
+  <si>
+    <t>testDeletes() sub-test 3</t>
+  </si>
+  <si>
+    <t>testInserts() sub-test 1</t>
+  </si>
+  <si>
+    <t>testInserts() sub-test 2</t>
+  </si>
+  <si>
+    <t>testInserts() sub-test 3</t>
+  </si>
+  <si>
+    <t>testInserts() sub-test 4</t>
+  </si>
+  <si>
+    <t>testUpdates() sub-test 1</t>
+  </si>
+  <si>
+    <t>testUpdates() sub-test 2</t>
+  </si>
+  <si>
+    <t>Content Provider (SQLite) tests:</t>
+  </si>
+  <si>
+    <t>Check if all data in the entry is correct.</t>
+  </si>
+  <si>
+    <t>"DrinkTable" should contain only one Drink.</t>
+  </si>
+  <si>
+    <t>Inserts one Drink into the table: "DrinkTable" by using the Content Provider.</t>
+  </si>
+  <si>
+    <t>testInserts() sub-test 5</t>
+  </si>
+  <si>
+    <t>Try to insert a row that already exists. Should return an exception.</t>
+  </si>
+  <si>
+    <t>Moves to the first record with cursor. Should point to the first and only row.</t>
+  </si>
+  <si>
+    <t>Try to delete an empty record.</t>
+  </si>
+  <si>
+    <t>Delete an existing record.</t>
+  </si>
+  <si>
+    <t>Check if the row was actually deleted.</t>
+  </si>
+  <si>
+    <t>Try to update an empty record.</t>
+  </si>
+  <si>
+    <t>Update an existing record.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned no exceptions.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned one row from table.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned correct data.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned an exception.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned zero rows deleted.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned one row deleted.</t>
+  </si>
+  <si>
+    <t>PASSED! Query and check that cursor.getCount returns zero.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned zero rows updated.</t>
+  </si>
+  <si>
+    <t>PASSED! Returned one row updated.</t>
   </si>
 </sst>
 </file>
@@ -350,17 +440,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -374,7 +464,123 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>